<commit_message>
fix prep_palm_input_update.m script & output
</commit_message>
<xml_diff>
--- a/code/h1_data_right.xlsx
+++ b/code/h1_data_right.xlsx
@@ -10,6 +10,53 @@
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>IV_avg</t>
+  </si>
+  <si>
+    <t>V_avg</t>
+  </si>
+  <si>
+    <t>VI_avg</t>
+  </si>
+  <si>
+    <t>Crus_I_avg</t>
+  </si>
+  <si>
+    <t>Crus_II_avg</t>
+  </si>
+  <si>
+    <t>VIIb_avg</t>
+  </si>
+  <si>
+    <t>VIIIa_avg</t>
+  </si>
+  <si>
+    <t>VIIIb_avg</t>
+  </si>
+  <si>
+    <t>IX_avg</t>
+  </si>
+  <si>
+    <t>X_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VI_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIa_avg</t>
+  </si>
+  <si>
+    <t>Vermis_VIIIb_avg</t>
+  </si>
+  <si>
+    <t>Vermis_IX_avg</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53,22 +100,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR52"/>
+  <dimension ref="A1:BR53"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="true"/>
-    <col min="2" max="2" width="14.7109375" customWidth="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="true"/>
+    <col min="2" max="2" width="14.42578125" customWidth="true"/>
     <col min="3" max="3" width="14.42578125" customWidth="true"/>
-    <col min="4" max="4" width="15.42578125" customWidth="true"/>
-    <col min="5" max="5" width="14.42578125" customWidth="true"/>
-    <col min="6" max="6" width="14.42578125" customWidth="true"/>
-    <col min="7" max="7" width="14.7109375" customWidth="true"/>
-    <col min="8" max="8" width="14.42578125" customWidth="true"/>
-    <col min="9" max="9" width="14.42578125" customWidth="true"/>
-    <col min="10" max="10" width="14.42578125" customWidth="true"/>
-    <col min="11" max="11" width="15.5703125" customWidth="true"/>
-    <col min="12" max="12" width="15.42578125" customWidth="true"/>
-    <col min="13" max="13" width="14.7109375" customWidth="true"/>
+    <col min="4" max="4" width="14.42578125" customWidth="true"/>
+    <col min="5" max="5" width="15.42578125" customWidth="true"/>
+    <col min="6" max="6" width="16.42578125" customWidth="true"/>
+    <col min="7" max="7" width="16.42578125" customWidth="true"/>
+    <col min="8" max="8" width="15.42578125" customWidth="true"/>
+    <col min="9" max="9" width="15.42578125" customWidth="true"/>
+    <col min="10" max="10" width="15.42578125" customWidth="true"/>
+    <col min="11" max="11" width="14.7109375" customWidth="true"/>
+    <col min="12" max="12" width="16.42578125" customWidth="true"/>
+    <col min="13" max="13" width="16.5703125" customWidth="true"/>
     <col min="14" max="14" width="15.42578125" customWidth="true"/>
     <col min="15" max="15" width="14.42578125" customWidth="true"/>
     <col min="16" max="16" width="15.42578125" customWidth="true"/>
@@ -129,47 +176,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0">
-        <v>0.40139581540000002</v>
-      </c>
-      <c r="B1" s="0">
-        <v>0.59335746960000002</v>
-      </c>
-      <c r="C1" s="0">
-        <v>0</v>
-      </c>
-      <c r="D1" s="0">
-        <v>-0.26262065600000001</v>
-      </c>
-      <c r="E1" s="0">
-        <v>-0.032857592550000002</v>
-      </c>
-      <c r="F1" s="0">
-        <v>0.43763005789999998</v>
-      </c>
-      <c r="G1" s="0">
-        <v>0.20784464750000001</v>
-      </c>
-      <c r="H1" s="0">
-        <v>0</v>
-      </c>
-      <c r="I1" s="0">
-        <v>-0.02703139114</v>
-      </c>
-      <c r="J1" s="0">
-        <v>-0.75416275229999996</v>
-      </c>
-      <c r="K1" s="0">
-        <v>-0.34883616010000001</v>
-      </c>
-      <c r="L1" s="0">
-        <v>0.54172162540000002</v>
-      </c>
-      <c r="M1" s="0">
-        <v>0</v>
-      </c>
-      <c r="N1" s="0">
-        <v>-0.25819401060000002</v>
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="O1" s="0">
         <v>-0.36030029759999999</v>
@@ -342,46 +389,46 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>-0.67251381129999999</v>
+        <v>0.14078792467500001</v>
       </c>
       <c r="B2" s="0">
-        <v>-0.30129863880000002</v>
+        <v>0.26596551942999996</v>
       </c>
       <c r="C2" s="0">
-        <v>0</v>
+        <v>0.16630994242500002</v>
       </c>
       <c r="D2" s="0">
-        <v>0.54700750570000001</v>
+        <v>-0.10697171619500001</v>
       </c>
       <c r="E2" s="0">
-        <v>-1.0526722180000001</v>
+        <v>0.078230294397499983</v>
       </c>
       <c r="F2" s="0">
-        <v>-0.36819422759999998</v>
+        <v>0.3620132902</v>
       </c>
       <c r="G2" s="0">
-        <v>-0.32645735120000002</v>
+        <v>0.45045286733250001</v>
       </c>
       <c r="H2" s="0">
-        <v>0</v>
+        <v>0.051652257710499999</v>
       </c>
       <c r="I2" s="0">
-        <v>0.11397211760000001</v>
+        <v>0.23966917888525002</v>
       </c>
       <c r="J2" s="0">
-        <v>-1.1965009900000001</v>
+        <v>-0.39799031565000004</v>
       </c>
       <c r="K2" s="0">
-        <v>-0.78920822810000002</v>
+        <v>0.37361356288500003</v>
       </c>
       <c r="L2" s="0">
-        <v>-0.06126496427</v>
+        <v>0.77566791997499995</v>
       </c>
       <c r="M2" s="0">
-        <v>0</v>
+        <v>0.35305775685000002</v>
       </c>
       <c r="N2" s="0">
-        <v>-0.0040876548900000004</v>
+        <v>0.58037688677499999</v>
       </c>
       <c r="O2" s="0">
         <v>-2.2181104129999998</v>
@@ -554,46 +601,46 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>-0.045589361830000001</v>
+        <v>-0.20996722792500003</v>
       </c>
       <c r="B3" s="0">
-        <v>0.93883183079999999</v>
+        <v>-0.37201425342500005</v>
       </c>
       <c r="C3" s="0">
-        <v>0.36163227930000003</v>
+        <v>-0.61009833860000007</v>
       </c>
       <c r="D3" s="0">
-        <v>0.493570913</v>
+        <v>-0.19790024845000001</v>
       </c>
       <c r="E3" s="0">
-        <v>0.25929785910000003</v>
+        <v>-0.49357198542499992</v>
       </c>
       <c r="F3" s="0">
-        <v>0.2485477281</v>
+        <v>-0.89110872922499995</v>
       </c>
       <c r="G3" s="0">
-        <v>0.35884231789999999</v>
+        <v>-0.32303606535000001</v>
       </c>
       <c r="H3" s="0">
-        <v>0.55041693069999997</v>
+        <v>-0.15099334535999998</v>
       </c>
       <c r="I3" s="0">
-        <v>0.39449871869999997</v>
+        <v>-0.58349606397499998</v>
       </c>
       <c r="J3" s="0">
-        <v>0.93802887430000004</v>
+        <v>0.15926253912500002</v>
       </c>
       <c r="K3" s="0">
-        <v>0.29917803129999998</v>
+        <v>-1.0817383018250002</v>
       </c>
       <c r="L3" s="0">
-        <v>0.1120985996</v>
+        <v>-0.61146063805000006</v>
       </c>
       <c r="M3" s="0">
-        <v>0.13761949279999999</v>
+        <v>0.017350899924999941</v>
       </c>
       <c r="N3" s="0">
-        <v>0.2418992204</v>
+        <v>-0.51186113249999998</v>
       </c>
       <c r="O3" s="0">
         <v>2.209751169</v>
@@ -766,46 +813,46 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.029054978669999999</v>
+        <v>0.011246142311999996</v>
       </c>
       <c r="B4" s="0">
-        <v>0.29736713650000002</v>
+        <v>0.091198319780000009</v>
       </c>
       <c r="C4" s="0">
-        <v>-0.27950413959999998</v>
+        <v>0.42554838991599997</v>
       </c>
       <c r="D4" s="0">
-        <v>0</v>
+        <v>0.2966529564</v>
       </c>
       <c r="E4" s="0">
-        <v>0.33902394650000001</v>
+        <v>-0.00039751792000002338</v>
       </c>
       <c r="F4" s="0">
-        <v>-0.17578295520000001</v>
+        <v>0.12179037455999997</v>
       </c>
       <c r="G4" s="0">
-        <v>0.0052704878020000002</v>
+        <v>0.22271198225400002</v>
       </c>
       <c r="H4" s="0">
-        <v>-0.098158639529999994</v>
+        <v>0.24734662946800001</v>
       </c>
       <c r="I4" s="0">
-        <v>0</v>
+        <v>-0.0187820136116</v>
       </c>
       <c r="J4" s="0">
-        <v>0.0283401356</v>
+        <v>0.21327603598800002</v>
       </c>
       <c r="K4" s="0">
-        <v>0.46734508070000003</v>
+        <v>0.058380246290000007</v>
       </c>
       <c r="L4" s="0">
-        <v>0.15542970840000001</v>
+        <v>-0.50945415488000001</v>
       </c>
       <c r="M4" s="0">
-        <v>0.041483946450000003</v>
+        <v>-0.57936641748400008</v>
       </c>
       <c r="N4" s="0">
-        <v>0</v>
+        <v>-0.66729688630000017</v>
       </c>
       <c r="O4" s="0">
         <v>0.4165435166</v>
@@ -978,46 +1025,46 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.015241109940000001</v>
+        <v>-0.265790235185</v>
       </c>
       <c r="B5" s="0">
-        <v>-0.20937340509999999</v>
+        <v>-0.06316968052999998</v>
       </c>
       <c r="C5" s="0">
-        <v>-0.35177540280000003</v>
+        <v>-0.02475423363249999</v>
       </c>
       <c r="D5" s="0">
-        <v>0.24674566319999999</v>
+        <v>-0.115945025625</v>
       </c>
       <c r="E5" s="0">
-        <v>-0.42912639250000001</v>
+        <v>-0.029614134842500001</v>
       </c>
       <c r="F5" s="0">
-        <v>-0.063943064460000004</v>
+        <v>-0.1670532945</v>
       </c>
       <c r="G5" s="0">
-        <v>0.31974871049999998</v>
+        <v>-0.33613959226750001</v>
       </c>
       <c r="H5" s="0">
-        <v>-0.47604503660000003</v>
+        <v>-0.21393806663749998</v>
       </c>
       <c r="I5" s="0">
-        <v>0.46976384739999999</v>
+        <v>0.24070038344</v>
       </c>
       <c r="J5" s="0">
-        <v>-0.080917237650000001</v>
+        <v>0.24815848730000001</v>
       </c>
       <c r="K5" s="0">
-        <v>-0.20217076549999999</v>
+        <v>0.12100199635000002</v>
       </c>
       <c r="L5" s="0">
-        <v>0.38404821420000002</v>
+        <v>-0.016418232725000009</v>
       </c>
       <c r="M5" s="0">
-        <v>-0.25713706660000002</v>
+        <v>0.064603163825000004</v>
       </c>
       <c r="N5" s="0">
-        <v>0.3787432698</v>
+        <v>0.35563680199250003</v>
       </c>
       <c r="O5" s="0">
         <v>0.041952293760000002</v>
@@ -1190,46 +1237,46 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.4610807723</v>
+        <v>0.075152260453999989</v>
       </c>
       <c r="B6" s="0">
-        <v>-0.38813394130000001</v>
+        <v>-0.083660592499999992</v>
       </c>
       <c r="C6" s="0">
-        <v>-0.98765660489999996</v>
+        <v>-0.062494528991999976</v>
       </c>
       <c r="D6" s="0">
-        <v>0.12742799290000001</v>
+        <v>0.12776610860200002</v>
       </c>
       <c r="E6" s="0">
-        <v>0.07301219062</v>
+        <v>0.28439010749999999</v>
       </c>
       <c r="F6" s="0">
-        <v>0.79147225830000001</v>
+        <v>0.207493784958</v>
       </c>
       <c r="G6" s="0">
-        <v>-0.11277357490000001</v>
+        <v>0.14752463677399999</v>
       </c>
       <c r="H6" s="0">
-        <v>-1.015825974</v>
+        <v>-0.024887240086000007</v>
       </c>
       <c r="I6" s="0">
-        <v>-0.25532232420000001</v>
+        <v>0.25218266547199997</v>
       </c>
       <c r="J6" s="0">
-        <v>0.2030372134</v>
+        <v>0.02003721643999996</v>
       </c>
       <c r="K6" s="0">
-        <v>0.54374291220000004</v>
+        <v>0.41747833310000004</v>
       </c>
       <c r="L6" s="0">
-        <v>-0.61160153490000002</v>
+        <v>0.22016945222000001</v>
       </c>
       <c r="M6" s="0">
-        <v>-1.151763589</v>
+        <v>0.197302110374</v>
       </c>
       <c r="N6" s="0">
-        <v>-0.102601216</v>
+        <v>0.22882967936000004</v>
       </c>
       <c r="O6" s="0">
         <v>0.36606569439999997</v>
@@ -1402,46 +1449,46 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>-1.2071308780000001</v>
+        <v>-0.046250182824200001</v>
       </c>
       <c r="B7" s="0">
-        <v>-0.50451900329999999</v>
+        <v>-0.058722906380000009</v>
       </c>
       <c r="C7" s="0">
-        <v>0.1707058615</v>
+        <v>0.10204974968</v>
       </c>
       <c r="D7" s="0">
-        <v>-0.78544971480000003</v>
+        <v>0.16056402572400003</v>
       </c>
       <c r="E7" s="0">
-        <v>-0.46171579569999999</v>
+        <v>0.063559975859999979</v>
       </c>
       <c r="F7" s="0">
-        <v>-1.159274827</v>
+        <v>0.051341626019999996</v>
       </c>
       <c r="G7" s="0">
-        <v>-1.041242663</v>
+        <v>0.17964860281999998</v>
       </c>
       <c r="H7" s="0">
-        <v>0.74775663950000004</v>
+        <v>-0.205075073</v>
       </c>
       <c r="I7" s="0">
-        <v>-1.0101950319999999</v>
+        <v>-0.28404945481799998</v>
       </c>
       <c r="J7" s="0">
-        <v>-0.45341152169999999</v>
+        <v>-0.19861942588000001</v>
       </c>
       <c r="K7" s="0">
-        <v>-1.229076506</v>
+        <v>-0.18115958201999999</v>
       </c>
       <c r="L7" s="0">
-        <v>-0.71791726199999994</v>
+        <v>0.17239634705999998</v>
       </c>
       <c r="M7" s="0">
-        <v>0.38414495430000001</v>
+        <v>-0.010100408779999992</v>
       </c>
       <c r="N7" s="0">
-        <v>-1.0001437259999999</v>
+        <v>0.054758378799999986</v>
       </c>
       <c r="O7" s="0">
         <v>-0.56850860540000003</v>
@@ -1614,46 +1661,46 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.48755488790000001</v>
+        <v>-0.44372081094000004</v>
       </c>
       <c r="B8" s="0">
-        <v>0.78673533929999995</v>
+        <v>-0.40098112718000001</v>
       </c>
       <c r="C8" s="0">
-        <v>0.64391636360000004</v>
+        <v>-0.54660805333999996</v>
       </c>
       <c r="D8" s="0">
-        <v>0.2367930261</v>
+        <v>-0.334807986286</v>
       </c>
       <c r="E8" s="0">
-        <v>0.27222956609999999</v>
+        <v>-0.48509310258000005</v>
       </c>
       <c r="F8" s="0">
-        <v>0.33531898040000002</v>
+        <v>-0.38045419493400001</v>
       </c>
       <c r="G8" s="0">
-        <v>0.3381699957</v>
+        <v>-0.22839825474</v>
       </c>
       <c r="H8" s="0">
-        <v>0.1409513154</v>
+        <v>-0.20601011471200001</v>
       </c>
       <c r="I8" s="0">
-        <v>0.48696700040000002</v>
+        <v>-0.49849447953799997</v>
       </c>
       <c r="J8" s="0">
-        <v>0.48823011519999998</v>
+        <v>-0.65786008768600002</v>
       </c>
       <c r="K8" s="0">
-        <v>-0.23493276690000001</v>
+        <v>-0.71668320002000008</v>
       </c>
       <c r="L8" s="0">
-        <v>-0.076455056940000002</v>
+        <v>-0.72865651773999995</v>
       </c>
       <c r="M8" s="0">
-        <v>0.51999920249999998</v>
+        <v>-0.74729739013999996</v>
       </c>
       <c r="N8" s="0">
-        <v>-0.026515218359999999</v>
+        <v>-1.0532261623600001</v>
       </c>
       <c r="O8" s="0">
         <v>0.26118116409999997</v>
@@ -1826,46 +1873,46 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>-0.25055478050000002</v>
+        <v>0.036879565980000008</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.7491033829</v>
+        <v>-0.064233556012599988</v>
       </c>
       <c r="C9" s="0">
-        <v>0.86169241249999995</v>
+        <v>-0.11040672753599998</v>
       </c>
       <c r="D9" s="0">
-        <v>-0.56279399959999998</v>
+        <v>-0.50877844657600002</v>
       </c>
       <c r="E9" s="0">
-        <v>0.37016882719999999</v>
+        <v>-0.37404365519599997</v>
       </c>
       <c r="F9" s="0">
-        <v>-0.58766417920000003</v>
+        <v>-0.18374198442999998</v>
       </c>
       <c r="G9" s="0">
-        <v>-0.67713943619999994</v>
+        <v>-0.35802148322000005</v>
       </c>
       <c r="H9" s="0">
-        <v>0.76880250959999996</v>
+        <v>-0.28461735014599998</v>
       </c>
       <c r="I9" s="0">
-        <v>-0.83649980239999999</v>
+        <v>-0.072612520740000047</v>
       </c>
       <c r="J9" s="0">
-        <v>0.65784015760000003</v>
+        <v>-0.66241787896000004</v>
       </c>
       <c r="K9" s="0">
-        <v>-0.51291400470000004</v>
+        <v>0.62180340515999999</v>
       </c>
       <c r="L9" s="0">
-        <v>-0.52608365130000001</v>
+        <v>-0.30348870484000001</v>
       </c>
       <c r="M9" s="0">
-        <v>0.76652870500000003</v>
+        <v>0.21463355250399996</v>
       </c>
       <c r="N9" s="0">
-        <v>-0.95812173379999999</v>
+        <v>0.031344307233999988</v>
       </c>
       <c r="O9" s="0">
         <v>1.475594625</v>
@@ -2038,46 +2085,46 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.58013587710000003</v>
+        <v>-0.16357386251999997</v>
       </c>
       <c r="B10" s="0">
-        <v>0.57677214730000004</v>
+        <v>-0.38012091135999998</v>
       </c>
       <c r="C10" s="0">
-        <v>0.4133965584</v>
+        <v>-0.36911390267999999</v>
       </c>
       <c r="D10" s="0">
-        <v>0.57262889630000002</v>
+        <v>-0.21916933635999997</v>
       </c>
       <c r="E10" s="0">
-        <v>-0.165548638</v>
+        <v>-0.30566488081999998</v>
       </c>
       <c r="F10" s="0">
-        <v>0.96923663120000003</v>
+        <v>-0.14736685736400004</v>
       </c>
       <c r="G10" s="0">
-        <v>0.63719608120000004</v>
+        <v>-0.36368383753799993</v>
       </c>
       <c r="H10" s="0">
-        <v>0.394744651</v>
+        <v>-0.30805091755199998</v>
       </c>
       <c r="I10" s="0">
-        <v>1.205778367</v>
+        <v>-0.36888629785999999</v>
       </c>
       <c r="J10" s="0">
-        <v>-0.074621501990000005</v>
+        <v>-0.34913975616600001</v>
       </c>
       <c r="K10" s="0">
-        <v>0.48310562109999999</v>
+        <v>-0.2811325241</v>
       </c>
       <c r="L10" s="0">
-        <v>0.101713257</v>
+        <v>-0.25616873369800003</v>
       </c>
       <c r="M10" s="0">
-        <v>0.038194990579999998</v>
+        <v>-0.14783237815199998</v>
       </c>
       <c r="N10" s="0">
-        <v>0.078986582520000001</v>
+        <v>-0.21109517222000002</v>
       </c>
       <c r="O10" s="0">
         <v>0.076811407009999999</v>
@@ -2250,46 +2297,46 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>-0.195762782</v>
+        <v>0.43902604907999992</v>
       </c>
       <c r="B11" s="0">
-        <v>0.007631197476</v>
+        <v>0.62174968051399992</v>
       </c>
       <c r="C11" s="0">
-        <v>-0.3320958316</v>
+        <v>0.002251029839999974</v>
       </c>
       <c r="D11" s="0">
-        <v>0.31411152990000002</v>
+        <v>-0.04867447251600001</v>
       </c>
       <c r="E11" s="0">
-        <v>-0.3438927987</v>
+        <v>-0.022138395179999992</v>
       </c>
       <c r="F11" s="0">
-        <v>-0.2024069329</v>
+        <v>0.0047877875659999569</v>
       </c>
       <c r="G11" s="0">
-        <v>-0.11652953169999999</v>
+        <v>-0.26898757822000002</v>
       </c>
       <c r="H11" s="0">
-        <v>0.42071758840000001</v>
+        <v>0.061678997759999986</v>
       </c>
       <c r="I11" s="0">
-        <v>0.06015679644</v>
+        <v>-0.018555769572000006</v>
       </c>
       <c r="J11" s="0">
-        <v>-0.38328148870000001</v>
+        <v>-0.050805510733999991</v>
       </c>
       <c r="K11" s="0">
-        <v>0.1192880601</v>
+        <v>-0.40895341122000001</v>
       </c>
       <c r="L11" s="0">
-        <v>0.18762940689999999</v>
+        <v>-0.12527591523999998</v>
       </c>
       <c r="M11" s="0">
-        <v>-0.015444590419999999</v>
+        <v>-0.29077796502000003</v>
       </c>
       <c r="N11" s="0">
-        <v>-0.53009159849999998</v>
+        <v>0.10336844882199998</v>
       </c>
       <c r="O11" s="0">
         <v>-0.47033640300000001</v>
@@ -2462,46 +2509,46 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>-0.2011932031</v>
+        <v>-0.15845044899999999</v>
       </c>
       <c r="B12" s="0">
-        <v>0.18558147820000001</v>
+        <v>-0.27926780021200004</v>
       </c>
       <c r="C12" s="0">
-        <v>-0.1636642247</v>
+        <v>-0.59725026784000002</v>
       </c>
       <c r="D12" s="0">
-        <v>0.16730130500000001</v>
+        <v>-0.059754489328000003</v>
       </c>
       <c r="E12" s="0">
-        <v>0.77530592180000002</v>
+        <v>0.19551790424000001</v>
       </c>
       <c r="F12" s="0">
-        <v>-0.8068307482</v>
+        <v>0.03885638120599999</v>
       </c>
       <c r="G12" s="0">
-        <v>0.20343617829999999</v>
+        <v>-0.29320587951999999</v>
       </c>
       <c r="H12" s="0">
-        <v>0.23346463840000001</v>
+        <v>-0.32984070730199999</v>
       </c>
       <c r="I12" s="0">
-        <v>0.043758825080000001</v>
+        <v>-0.23668373237399995</v>
       </c>
       <c r="J12" s="0">
-        <v>0.46739215589999999</v>
+        <v>-0.35530480878999998</v>
       </c>
       <c r="K12" s="0">
-        <v>-0.64823943439999998</v>
+        <v>-0.28550896895199995</v>
       </c>
       <c r="L12" s="0">
-        <v>0.56856668749999995</v>
+        <v>-0.25037050088399998</v>
       </c>
       <c r="M12" s="0">
-        <v>0.086545144439999999</v>
+        <v>-0.18137218692400001</v>
       </c>
       <c r="N12" s="0">
-        <v>0.61102869650000002</v>
+        <v>-0.56908704440000002</v>
       </c>
       <c r="O12" s="0">
         <v>0.24583915889999999</v>
@@ -2674,46 +2721,46 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>-0.8758120023</v>
+        <v>0.30051822974799997</v>
       </c>
       <c r="B13" s="0">
-        <v>0.49921846320000002</v>
+        <v>0.13337583942</v>
       </c>
       <c r="C13" s="0">
-        <v>0.306073225</v>
+        <v>0.25220422283400001</v>
       </c>
       <c r="D13" s="0">
-        <v>0.1735666749</v>
+        <v>0.30396299495950002</v>
       </c>
       <c r="E13" s="0">
-        <v>-0.1014700664</v>
+        <v>0.27963150699660005</v>
       </c>
       <c r="F13" s="0">
-        <v>-0.55432043539999998</v>
+        <v>0.1763784175</v>
       </c>
       <c r="G13" s="0">
-        <v>0.91845257560000004</v>
+        <v>0.12031741795999999</v>
       </c>
       <c r="H13" s="0">
-        <v>0.71219798990000005</v>
+        <v>0.083529181979999992</v>
       </c>
       <c r="I13" s="0">
-        <v>-0.42298617840000002</v>
+        <v>0.0029332390199999893</v>
       </c>
       <c r="J13" s="0">
-        <v>-0.086329381080000003</v>
+        <v>-0.26878169651999995</v>
       </c>
       <c r="K13" s="0">
-        <v>-0.86421503030000002</v>
+        <v>-0.16085545205999999</v>
       </c>
       <c r="L13" s="0">
-        <v>0.97035083450000004</v>
+        <v>0.018342300159999981</v>
       </c>
       <c r="M13" s="0">
-        <v>0.65346681470000001</v>
+        <v>0.33203034508000001</v>
       </c>
       <c r="N13" s="0">
-        <v>-0.1207171207</v>
+        <v>0.042822212560000003</v>
       </c>
       <c r="O13" s="0">
         <v>-0.33513325440000002</v>
@@ -2886,46 +2933,46 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.13061387190000001</v>
+        <v>0.011303165178000002</v>
       </c>
       <c r="B14" s="0">
-        <v>-0.99810639430000003</v>
+        <v>-0.19634436159999999</v>
       </c>
       <c r="C14" s="0">
-        <v>-0.32525532359999998</v>
+        <v>-0.16232105578</v>
       </c>
       <c r="D14" s="0">
-        <v>0.22977137559999999</v>
+        <v>-0.10306530106</v>
       </c>
       <c r="E14" s="0">
-        <v>-0.039689733919999998</v>
+        <v>-0.22192712380000001</v>
       </c>
       <c r="F14" s="0">
-        <v>-0.050933843030000002</v>
+        <v>-0.13984563656000001</v>
       </c>
       <c r="G14" s="0">
-        <v>-0.48662524159999998</v>
+        <v>-0.15166059926</v>
       </c>
       <c r="H14" s="0">
-        <v>-0.34681083540000002</v>
+        <v>0.15729562760599999</v>
       </c>
       <c r="I14" s="0">
-        <v>-0.4077806719</v>
+        <v>-0.051519462879999998</v>
       </c>
       <c r="J14" s="0">
-        <v>-0.1880594749</v>
+        <v>-0.082932634757999987</v>
       </c>
       <c r="K14" s="0">
-        <v>2.3307718009999999e-06</v>
+        <v>-0.31325015218000002</v>
       </c>
       <c r="L14" s="0">
-        <v>-0.099720159380000006</v>
+        <v>0.11465377557999998</v>
       </c>
       <c r="M14" s="0">
-        <v>0.24378479289999999</v>
+        <v>0.28574901727000002</v>
       </c>
       <c r="N14" s="0">
-        <v>-0.64037891830000004</v>
+        <v>-0.171643545738</v>
       </c>
       <c r="O14" s="0">
         <v>-0.21128192139999999</v>
@@ -3098,46 +3145,46 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.96831720310000002</v>
+        <v>-0.11704833063219999</v>
       </c>
       <c r="B15" s="0">
-        <v>-0.53717949850000002</v>
+        <v>-0.41955302310799991</v>
       </c>
       <c r="C15" s="0">
-        <v>-0.245666512</v>
+        <v>-0.43348702118800003</v>
       </c>
       <c r="D15" s="0">
-        <v>-0.20077098769999999</v>
+        <v>-0.30481580322000001</v>
       </c>
       <c r="E15" s="0">
-        <v>0.054949621999999997</v>
+        <v>-0.221646914498</v>
       </c>
       <c r="F15" s="0">
-        <v>0.92136447590000004</v>
+        <v>-0.13184560894000003</v>
       </c>
       <c r="G15" s="0">
-        <v>-0.7048370384</v>
+        <v>-0.077638379267999991</v>
       </c>
       <c r="H15" s="0">
-        <v>-0.1652442647</v>
+        <v>-0.079360108319999997</v>
       </c>
       <c r="I15" s="0">
-        <v>-0.59559636120000004</v>
+        <v>-0.21102132151199998</v>
       </c>
       <c r="J15" s="0">
-        <v>0.17412021659999999</v>
+        <v>0.18540586064600001</v>
       </c>
       <c r="K15" s="0">
-        <v>0.78694663580000002</v>
+        <v>-0.35782008699999995</v>
       </c>
       <c r="L15" s="0">
-        <v>-0.43015226350000002</v>
+        <v>-0.23205362875999999</v>
       </c>
       <c r="M15" s="0">
-        <v>0.0092821399140000007</v>
+        <v>-0.11742046106000001</v>
       </c>
       <c r="N15" s="0">
-        <v>-0.19141605240000001</v>
+        <v>-0.36712546653400013</v>
       </c>
       <c r="O15" s="0">
         <v>-0.40024857470000003</v>
@@ -3310,46 +3357,46 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>-0.25601499500000002</v>
+        <v>-0.163864794896</v>
       </c>
       <c r="B16" s="0">
-        <v>-0.29568902740000003</v>
+        <v>-0.45257119024000003</v>
       </c>
       <c r="C16" s="0">
-        <v>-0.30774166629999999</v>
+        <v>-0.24289018169999999</v>
       </c>
       <c r="D16" s="0">
-        <v>0.48082191569999999</v>
+        <v>-0.15225780405999997</v>
       </c>
       <c r="E16" s="0">
-        <v>0.26410165340000002</v>
+        <v>-0.0045503008200000082</v>
       </c>
       <c r="F16" s="0">
-        <v>-0.60919847250000003</v>
+        <v>-0.12429446513999998</v>
       </c>
       <c r="G16" s="0">
-        <v>-0.4063743071</v>
+        <v>-0.19612327743999999</v>
       </c>
       <c r="H16" s="0">
-        <v>-0.48599133839999997</v>
+        <v>-0.0080970890539999833</v>
       </c>
       <c r="I16" s="0">
-        <v>-0.036313552169999999</v>
+        <v>-0.0033179562679999997</v>
       </c>
       <c r="J16" s="0">
-        <v>0.41302751230000001</v>
+        <v>-0.34191488458000008</v>
       </c>
       <c r="K16" s="0">
-        <v>-0.32929951229999999</v>
+        <v>0.23085321906200001</v>
       </c>
       <c r="L16" s="0">
-        <v>-0.51672494899999999</v>
+        <v>0.12091792623999997</v>
       </c>
       <c r="M16" s="0">
-        <v>-0.34854410209999998</v>
+        <v>-0.0019727102000000052</v>
       </c>
       <c r="N16" s="0">
-        <v>-0.2638387298</v>
+        <v>-0.36020074282000003</v>
       </c>
       <c r="O16" s="0">
         <v>0.46355693100000001</v>
@@ -3522,46 +3569,46 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.44155907379999998</v>
+        <v>0.06157246027600001</v>
       </c>
       <c r="B17" s="0">
-        <v>0.25935341360000003</v>
+        <v>0.32655285828000002</v>
       </c>
       <c r="C17" s="0">
-        <v>-1.0646199750000001</v>
+        <v>0.05813387593599998</v>
       </c>
       <c r="D17" s="0">
-        <v>1.304537952</v>
+        <v>-0.06732317157999998</v>
       </c>
       <c r="E17" s="0">
-        <v>0</v>
+        <v>-0.111642629876</v>
       </c>
       <c r="F17" s="0">
-        <v>-0.1066802827</v>
+        <v>0.28014878629399997</v>
       </c>
       <c r="G17" s="0">
-        <v>0.40328224109999999</v>
+        <v>0.16924211245999998</v>
       </c>
       <c r="H17" s="0">
-        <v>-0.5366608195</v>
+        <v>-0.093072101560000009</v>
       </c>
       <c r="I17" s="0">
-        <v>0.69328915899999999</v>
+        <v>0.0026846111799999849</v>
       </c>
       <c r="J17" s="0">
-        <v>0</v>
+        <v>0.010436505385999995</v>
       </c>
       <c r="K17" s="0">
-        <v>0.17163606249999999</v>
+        <v>-0.068670296480000032</v>
       </c>
       <c r="L17" s="0">
-        <v>0.24422877700000001</v>
+        <v>0.02719032404599997</v>
       </c>
       <c r="M17" s="0">
-        <v>-0.1028440105</v>
+        <v>0.50373938381999994</v>
       </c>
       <c r="N17" s="0">
-        <v>0.73052144139999997</v>
+        <v>0.18934984831999996</v>
       </c>
       <c r="O17" s="0">
         <v>0</v>
@@ -3734,46 +3781,46 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.0013241041329999999</v>
+        <v>0.021125414995000008</v>
       </c>
       <c r="B18" s="0">
-        <v>-0.65615994320000004</v>
+        <v>-0.18004715732500001</v>
       </c>
       <c r="C18" s="0">
-        <v>0.33993802960000002</v>
+        <v>-0.0124531845925</v>
       </c>
       <c r="D18" s="0">
-        <v>-0.24524212840000001</v>
+        <v>-0.038457621994999996</v>
       </c>
       <c r="E18" s="0">
-        <v>0</v>
+        <v>-0.23062697845000002</v>
       </c>
       <c r="F18" s="0">
-        <v>-0.37854743219999998</v>
+        <v>-0.16930596272500001</v>
       </c>
       <c r="G18" s="0">
-        <v>-0.49013856099999997</v>
+        <v>0.02551024525249998</v>
       </c>
       <c r="H18" s="0">
-        <v>0.204566145</v>
+        <v>0.031910031836500014</v>
       </c>
       <c r="I18" s="0">
-        <v>-0.74900835030000001</v>
+        <v>-0.10878864083000001</v>
       </c>
       <c r="J18" s="0">
-        <v>0</v>
+        <v>0.12205327093574998</v>
       </c>
       <c r="K18" s="0">
-        <v>-0.21310105500000001</v>
+        <v>-0.26889287422499997</v>
       </c>
       <c r="L18" s="0">
-        <v>-0.64272883920000001</v>
+        <v>-0.32916763885</v>
       </c>
       <c r="M18" s="0">
-        <v>0.41988202920000001</v>
+        <v>0.24361328142500002</v>
       </c>
       <c r="N18" s="0">
-        <v>-0.38752540219999998</v>
+        <v>0.36766515242499997</v>
       </c>
       <c r="O18" s="0">
         <v>0</v>
@@ -3946,46 +3993,46 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.40604522999999998</v>
+        <v>-0.086102740804999994</v>
       </c>
       <c r="B19" s="0">
-        <v>0.39386306170000002</v>
+        <v>-0.36919370547499997</v>
       </c>
       <c r="C19" s="0">
-        <v>0.1306335079</v>
+        <v>-0.33390679635000003</v>
       </c>
       <c r="D19" s="0">
-        <v>-0.57399754150000004</v>
+        <v>-0.21369957297499997</v>
       </c>
       <c r="E19" s="0">
-        <v>-0.04507066941</v>
+        <v>0.1958148488375</v>
       </c>
       <c r="F19" s="0">
-        <v>-0.028857382210000001</v>
+        <v>-0.00029785093249999096</v>
       </c>
       <c r="G19" s="0">
-        <v>0.5627389787</v>
+        <v>-0.29794626537499996</v>
       </c>
       <c r="H19" s="0">
-        <v>-0.028685930080000002</v>
+        <v>-0.21076157285000002</v>
       </c>
       <c r="I19" s="0">
-        <v>-0.52135276109999995</v>
+        <v>-0.17427292932499999</v>
       </c>
       <c r="J19" s="0">
-        <v>-0.35732881630000002</v>
+        <v>-0.90753095297499997</v>
       </c>
       <c r="K19" s="0">
-        <v>0.50874581419999998</v>
+        <v>-0.31283989875000001</v>
       </c>
       <c r="L19" s="0">
-        <v>0.50109687650000001</v>
+        <v>-0.45975636275000004</v>
       </c>
       <c r="M19" s="0">
-        <v>-0.35131935939999998</v>
+        <v>-0.24084082355000003</v>
       </c>
       <c r="N19" s="0">
-        <v>-0.59902102530000001</v>
+        <v>-0.039308802249999997</v>
       </c>
       <c r="O19" s="0">
         <v>-0.075442163889999997</v>
@@ -4158,46 +4205,46 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.26797722950000002</v>
+        <v>0.14451395484000001</v>
       </c>
       <c r="B20" s="0">
-        <v>0.054403537260000003</v>
+        <v>0.17043902871400002</v>
       </c>
       <c r="C20" s="0">
-        <v>-0.25670443279999999</v>
+        <v>0.10241985370399997</v>
       </c>
       <c r="D20" s="0">
-        <v>-0.5847577853</v>
+        <v>-0.082397305899999995</v>
       </c>
       <c r="E20" s="0">
-        <v>-0.049274275309999997</v>
+        <v>0.022922990019999999</v>
       </c>
       <c r="F20" s="0">
-        <v>0.29220825179999999</v>
+        <v>-0.14732471937200001</v>
       </c>
       <c r="G20" s="0">
-        <v>-0.16952059259999999</v>
+        <v>-0.34707047121199996</v>
       </c>
       <c r="H20" s="0">
-        <v>-0.76920432999999999</v>
+        <v>-0.29321269420599994</v>
       </c>
       <c r="I20" s="0">
-        <v>-0.50567960710000004</v>
+        <v>0.063502752419999989</v>
       </c>
       <c r="J20" s="0">
-        <v>-0.3812074574</v>
+        <v>-0.32747274956</v>
       </c>
       <c r="K20" s="0">
-        <v>0.07640439769</v>
+        <v>0.41330670352599996</v>
       </c>
       <c r="L20" s="0">
-        <v>-0.15404597980000001</v>
+        <v>0.098217996520000003</v>
       </c>
       <c r="M20" s="0">
-        <v>-1.0866479760000001</v>
+        <v>0.061819566079999999</v>
       </c>
       <c r="N20" s="0">
-        <v>-0.023816072800000001</v>
+        <v>0.25117686824599994</v>
       </c>
       <c r="O20" s="0">
         <v>-0.1009908342</v>
@@ -4370,46 +4417,46 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>-0.44712758850000001</v>
+        <v>0.14248950532199997</v>
       </c>
       <c r="B21" s="0">
-        <v>0.086462402320000006</v>
+        <v>0.10957933396000001</v>
       </c>
       <c r="C21" s="0">
-        <v>0.3677974752</v>
+        <v>-0.04698306724000003</v>
       </c>
       <c r="D21" s="0">
-        <v>0</v>
+        <v>0.089475553418807988</v>
       </c>
       <c r="E21" s="0">
-        <v>0.14610145020000001</v>
+        <v>0.11315879173999999</v>
       </c>
       <c r="F21" s="0">
-        <v>-0.4258289488</v>
+        <v>0.00045212031599999871</v>
       </c>
       <c r="G21" s="0">
-        <v>0.28147685080000001</v>
+        <v>-0.22909799363199998</v>
       </c>
       <c r="H21" s="0">
-        <v>0.50195834500000003</v>
+        <v>0.057861978550000005</v>
       </c>
       <c r="I21" s="0">
-        <v>0</v>
+        <v>0.13745205542</v>
       </c>
       <c r="J21" s="0">
-        <v>0.056238650860000003</v>
+        <v>0.0048570535800000255</v>
       </c>
       <c r="K21" s="0">
-        <v>0.074031482060000001</v>
+        <v>0.023613967320000005</v>
       </c>
       <c r="L21" s="0">
-        <v>0.27817783159999998</v>
+        <v>-0.10295946076000002</v>
       </c>
       <c r="M21" s="0">
-        <v>0.61144046959999998</v>
+        <v>-0.19244461726000001</v>
       </c>
       <c r="N21" s="0">
-        <v>0</v>
+        <v>-0.091326127019999953</v>
       </c>
       <c r="O21" s="0">
         <v>0.2490971401</v>
@@ -4582,46 +4629,46 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>-0.90453631840000004</v>
+        <v>0.080301184349999999</v>
       </c>
       <c r="B22" s="0">
-        <v>0</v>
+        <v>0.11121237717499999</v>
       </c>
       <c r="C22" s="0">
-        <v>0.15684140669999999</v>
+        <v>0.20053681873250001</v>
       </c>
       <c r="D22" s="0">
-        <v>0</v>
+        <v>0.253788400325</v>
       </c>
       <c r="E22" s="0">
-        <v>0.70286292989999999</v>
+        <v>0.117898349175</v>
       </c>
       <c r="F22" s="0">
-        <v>-1.412192248</v>
+        <v>-0.0067020142349999961</v>
       </c>
       <c r="G22" s="0">
-        <v>0</v>
+        <v>0.059401056890000012</v>
       </c>
       <c r="H22" s="0">
-        <v>0.18739984170000001</v>
+        <v>0.090873267039000005</v>
       </c>
       <c r="I22" s="0">
-        <v>0</v>
+        <v>0.0022631391499999993</v>
       </c>
       <c r="J22" s="0">
-        <v>0.24701340299999999</v>
+        <v>0.21009968102500001</v>
       </c>
       <c r="K22" s="0">
-        <v>-1.2929541449999999</v>
+        <v>0.50044072319249999</v>
       </c>
       <c r="L22" s="0">
-        <v>0</v>
+        <v>0.17705848755000003</v>
       </c>
       <c r="M22" s="0">
-        <v>0.70005306069999995</v>
+        <v>0.14616942355499998</v>
       </c>
       <c r="N22" s="0">
-        <v>0</v>
+        <v>-0.12049259663499998</v>
       </c>
       <c r="O22" s="0">
         <v>0.112254042</v>
@@ -4794,46 +4841,46 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>-0.086526281770000005</v>
+        <v>-0.038742500723333295</v>
       </c>
       <c r="B23" s="0">
-        <v>0.088986706949999994</v>
+        <v>0.005606001400000042</v>
       </c>
       <c r="C23" s="0">
-        <v>0.21662189509999999</v>
+        <v>-0.25072066682333333</v>
       </c>
       <c r="D23" s="0">
-        <v>0.1129782943</v>
+        <v>-0.24637354443333334</v>
       </c>
       <c r="E23" s="0">
-        <v>-0.71186281699999998</v>
+        <v>-0.20972510433333333</v>
       </c>
       <c r="F23" s="0">
-        <v>0.44144316420000002</v>
+        <v>-0.064085606800000028</v>
       </c>
       <c r="G23" s="0">
-        <v>-0.55846579839999999</v>
+        <v>-0.00041695513333332251</v>
       </c>
       <c r="H23" s="0">
-        <v>0.089526340839999996</v>
+        <v>-0.14675637819999998</v>
       </c>
       <c r="I23" s="0">
-        <v>-0.55184611019999996</v>
+        <v>-0.11856402789999999</v>
       </c>
       <c r="J23" s="0">
-        <v>-0.91217811209999999</v>
+        <v>0.26910250366666666</v>
       </c>
       <c r="K23" s="0">
-        <v>0.40304665589999999</v>
+        <v>0.011863568666666676</v>
       </c>
       <c r="L23" s="0">
-        <v>0.1065676986</v>
+        <v>-0.25109867266166663</v>
       </c>
       <c r="M23" s="0">
-        <v>-0.31899064059999999</v>
+        <v>-0.55927359033333335</v>
       </c>
       <c r="N23" s="0">
-        <v>-0.75373231480000003</v>
+        <v>-0.56220660633333341</v>
       </c>
       <c r="O23" s="0">
         <v>-0.77191658500000004</v>
@@ -5006,46 +5053,46 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.079392492179999996</v>
+        <v>-0.10948256708</v>
       </c>
       <c r="B24" s="0">
-        <v>-0.17528578440000001</v>
+        <v>0.13888830173999997</v>
       </c>
       <c r="C24" s="0">
-        <v>-0.42785447259999998</v>
+        <v>-0.066237421699999979</v>
       </c>
       <c r="D24" s="0">
-        <v>0.025163551329999999</v>
+        <v>-0.14813689386000001</v>
       </c>
       <c r="E24" s="0">
-        <v>0.32854447520000002</v>
+        <v>-0.34964032880999996</v>
       </c>
       <c r="F24" s="0">
-        <v>0.1727453719</v>
+        <v>-0.33009275749599998</v>
       </c>
       <c r="G24" s="0">
-        <v>-0.027096188090000001</v>
+        <v>-0.267874583188</v>
       </c>
       <c r="H24" s="0">
-        <v>0.33835182089999999</v>
+        <v>-0.109783591922</v>
       </c>
       <c r="I24" s="0">
-        <v>0.072925568029999999</v>
+        <v>-0.15715466832399999</v>
       </c>
       <c r="J24" s="0">
-        <v>-0.02379636035</v>
+        <v>0.20344207060000002</v>
       </c>
       <c r="K24" s="0">
-        <v>0.110237601</v>
+        <v>-0.079265349780000022</v>
       </c>
       <c r="L24" s="0">
-        <v>0.4184824513</v>
+        <v>-0.039170010439999993</v>
       </c>
       <c r="M24" s="0">
-        <v>-0.27246737739999999</v>
+        <v>-0.2497478494</v>
       </c>
       <c r="N24" s="0">
-        <v>-0.1152114638</v>
+        <v>0.081565159547999991</v>
       </c>
       <c r="O24" s="0">
         <v>0.39063300579999999</v>
@@ -5218,46 +5265,46 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0</v>
+        <v>0.038499392198000006</v>
       </c>
       <c r="B25" s="0">
-        <v>0</v>
+        <v>0.073342423279999985</v>
       </c>
       <c r="C25" s="0">
-        <v>-0.58317379749999998</v>
+        <v>0.097716607004000006</v>
       </c>
       <c r="D25" s="0">
-        <v>0.1500619399</v>
+        <v>-0.10004688246</v>
       </c>
       <c r="E25" s="0">
-        <v>0.3902424491</v>
+        <v>-0.043297388674000001</v>
       </c>
       <c r="F25" s="0">
-        <v>0</v>
+        <v>0.087156541693999987</v>
       </c>
       <c r="G25" s="0">
-        <v>0</v>
+        <v>0.109150521236</v>
       </c>
       <c r="H25" s="0">
-        <v>-0.3176771229</v>
+        <v>0.056874350393999996</v>
       </c>
       <c r="I25" s="0">
-        <v>-0.071987901770000001</v>
+        <v>-0.081188785966000002</v>
       </c>
       <c r="J25" s="0">
-        <v>0.010051767079999999</v>
+        <v>0.37998423557999994</v>
       </c>
       <c r="K25" s="0">
-        <v>0</v>
+        <v>0.40660311591399995</v>
       </c>
       <c r="L25" s="0">
-        <v>0</v>
+        <v>-0.049990135681999996</v>
       </c>
       <c r="M25" s="0">
-        <v>-0.50176940869999997</v>
+        <v>-0.21499274298599999</v>
       </c>
       <c r="N25" s="0">
-        <v>-0.11442286760000001</v>
+        <v>-0.36169255513999998</v>
       </c>
       <c r="O25" s="0">
         <v>0.32989356390000002</v>
@@ -5430,46 +5477,46 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.38785974569999998</v>
+        <v>0.061502550999999996</v>
       </c>
       <c r="B26" s="0">
-        <v>-0.44996749549999998</v>
+        <v>0.0067346224899999989</v>
       </c>
       <c r="C26" s="0">
-        <v>-0.094541803490000006</v>
+        <v>-0.21923077198609997</v>
       </c>
       <c r="D26" s="0">
-        <v>0</v>
+        <v>0.0085273242399999949</v>
       </c>
       <c r="E26" s="0">
-        <v>-0.3758047967</v>
+        <v>-0.12654775467666665</v>
       </c>
       <c r="F26" s="0">
-        <v>0.2840467156</v>
+        <v>-0.41062985349999997</v>
       </c>
       <c r="G26" s="0">
-        <v>-0.43326500559999997</v>
+        <v>-0.4066954079666667</v>
       </c>
       <c r="H26" s="0">
-        <v>0.44105200039999998</v>
+        <v>-0.17251750024666668</v>
       </c>
       <c r="I26" s="0">
-        <v>0</v>
+        <v>-0.32537496252333337</v>
       </c>
       <c r="J26" s="0">
-        <v>-0.60653401969999998</v>
+        <v>0.037885950533333351</v>
       </c>
       <c r="K26" s="0">
-        <v>0.64426112329999996</v>
+        <v>-0.65188641840000006</v>
       </c>
       <c r="L26" s="0">
-        <v>-0.6664067776</v>
+        <v>-0.35387869519999998</v>
       </c>
       <c r="M26" s="0">
-        <v>0.15526049680000001</v>
+        <v>0.097853719126666669</v>
       </c>
       <c r="N26" s="0">
-        <v>0</v>
+        <v>-0.39325813067333332</v>
       </c>
       <c r="O26" s="0">
         <v>-0.038188072500000003</v>
@@ -5642,46 +5689,46 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>-0.0049425085059999997</v>
+        <v>0.26791140154999998</v>
       </c>
       <c r="B27" s="0">
-        <v>-0.52255196749999999</v>
+        <v>0.27317585794999999</v>
       </c>
       <c r="C27" s="0">
-        <v>-0.26409859899999999</v>
+        <v>0.25231569792499997</v>
       </c>
       <c r="D27" s="0">
-        <v>0.92210137709999995</v>
+        <v>-0.15601855989999996</v>
       </c>
       <c r="E27" s="0">
-        <v>-0.2378958441</v>
+        <v>-0.30020843548999998</v>
       </c>
       <c r="F27" s="0">
-        <v>-0.1314870356</v>
+        <v>0.073465759132500003</v>
       </c>
       <c r="G27" s="0">
-        <v>-0.83088356919999995</v>
+        <v>0.058305518022500002</v>
       </c>
       <c r="H27" s="0">
-        <v>-0.08973930058</v>
+        <v>-0.092860258884999977</v>
       </c>
       <c r="I27" s="0">
-        <v>1.1017132700000001</v>
+        <v>0.33534835292249998</v>
       </c>
       <c r="J27" s="0">
-        <v>-0.6090475246</v>
+        <v>0.10834539967499998</v>
       </c>
       <c r="K27" s="0">
-        <v>-0.072116391429999996</v>
+        <v>-0.031301431540000008</v>
       </c>
       <c r="L27" s="0">
-        <v>-0.32922618609999998</v>
+        <v>0.15127281110000002</v>
       </c>
       <c r="M27" s="0">
-        <v>0.1748357914</v>
+        <v>0.2165755597</v>
       </c>
       <c r="N27" s="0">
-        <v>1.2244188250000001</v>
+        <v>0.7588626394500001</v>
       </c>
       <c r="O27" s="0">
         <v>-0.61454732560000003</v>
@@ -5854,46 +5901,46 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>-0.29421582940000002</v>
+        <v>0.028689984535999989</v>
       </c>
       <c r="B28" s="0">
-        <v>-0.1285660525</v>
+        <v>-0.21070129789399999</v>
       </c>
       <c r="C28" s="0">
-        <v>0.22294938880000001</v>
+        <v>0.039537089235999988</v>
       </c>
       <c r="D28" s="0">
-        <v>0.3235297084</v>
+        <v>0.40224877119800001</v>
       </c>
       <c r="E28" s="0">
-        <v>-1.8674281319999999</v>
+        <v>0.54202843669600009</v>
       </c>
       <c r="F28" s="0">
-        <v>-0.040417653380000002</v>
+        <v>0.12840104280000003</v>
       </c>
       <c r="G28" s="0">
-        <v>0.15541317909999999</v>
+        <v>-0.25117204594199993</v>
       </c>
       <c r="H28" s="0">
-        <v>0.2703129823</v>
+        <v>-0.162105350334</v>
       </c>
       <c r="I28" s="0">
-        <v>0.2250050294</v>
+        <v>0.18447391130899998</v>
       </c>
       <c r="J28" s="0">
-        <v>-1.872235141</v>
+        <v>0.090551505599999998</v>
       </c>
       <c r="K28" s="0">
-        <v>-0.08929119613</v>
+        <v>0.001660866157999985</v>
       </c>
       <c r="L28" s="0">
-        <v>-0.38810195469999997</v>
+        <v>0.60506101535400003</v>
       </c>
       <c r="M28" s="0">
-        <v>0.084150002730000006</v>
+        <v>0.56499093984620008</v>
       </c>
       <c r="N28" s="0">
-        <v>0.26784253200000002</v>
+        <v>0.87886661916000008</v>
       </c>
       <c r="O28" s="0">
         <v>-0.53172428230000002</v>
@@ -6066,46 +6113,46 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>-0.55005639179999999</v>
+        <v>-0.37397472877999999</v>
       </c>
       <c r="B29" s="0">
-        <v>-0.33640054619999998</v>
+        <v>-0.23062598612000004</v>
       </c>
       <c r="C29" s="0">
-        <v>0.34150928219999999</v>
+        <v>-0.12107479055799997</v>
       </c>
       <c r="D29" s="0">
-        <v>-0.41484832259999999</v>
+        <v>-0.17289518916800001</v>
       </c>
       <c r="E29" s="0">
-        <v>0.18735566079999999</v>
+        <v>-0.31030802378</v>
       </c>
       <c r="F29" s="0">
-        <v>-0.2332984619</v>
+        <v>-0.35104926625599997</v>
       </c>
       <c r="G29" s="0">
-        <v>-0.18668026360000001</v>
+        <v>-0.10892573714000001</v>
       </c>
       <c r="H29" s="0">
-        <v>-0.3379539795</v>
+        <v>0.20946705527399997</v>
       </c>
       <c r="I29" s="0">
-        <v>0.036558273969999999</v>
+        <v>-0.10746744653999998</v>
       </c>
       <c r="J29" s="0">
-        <v>0.19079679220000001</v>
+        <v>-0.24744084557999999</v>
       </c>
       <c r="K29" s="0">
-        <v>0.02960920555</v>
+        <v>-0.29621993306</v>
       </c>
       <c r="L29" s="0">
-        <v>-0.2767923437</v>
+        <v>-0.42537753740000001</v>
       </c>
       <c r="M29" s="0">
-        <v>0.029112428360000001</v>
+        <v>-0.28426003882</v>
       </c>
       <c r="N29" s="0">
-        <v>-0.111181764</v>
+        <v>-0.032476712520000041</v>
       </c>
       <c r="O29" s="0">
         <v>0.168306397</v>
@@ -6278,46 +6325,46 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.2167759336</v>
+        <v>-0.10651011836799999</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.079447805960000006</v>
+        <v>-0.25213483841399997</v>
       </c>
       <c r="C30" s="0">
-        <v>0.13250946659999999</v>
+        <v>-0.031291007305600006</v>
       </c>
       <c r="D30" s="0">
-        <v>0.69961136049999995</v>
+        <v>0.140643875438</v>
       </c>
       <c r="E30" s="0">
-        <v>0.41512947519999999</v>
+        <v>0.1443385009</v>
       </c>
       <c r="F30" s="0">
-        <v>0.34307122029999998</v>
+        <v>-0.16326151867199998</v>
       </c>
       <c r="G30" s="0">
-        <v>0.057629381620000003</v>
+        <v>-0.24997396280199996</v>
       </c>
       <c r="H30" s="0">
-        <v>0.026772834820000001</v>
+        <v>-0.26821408975</v>
       </c>
       <c r="I30" s="0">
-        <v>0.10098940169999999</v>
+        <v>-0.058169491050000008</v>
       </c>
       <c r="J30" s="0">
-        <v>0.32341798300000002</v>
+        <v>0.51279745010200006</v>
       </c>
       <c r="K30" s="0">
-        <v>0.14179654089999999</v>
+        <v>0.064711638199999991</v>
       </c>
       <c r="L30" s="0">
-        <v>-0.16860522289999999</v>
+        <v>-0.13081929274399998</v>
       </c>
       <c r="M30" s="0">
-        <v>-0.47021649180000002</v>
+        <v>-0.010847766560000005</v>
       </c>
       <c r="N30" s="0">
-        <v>0.44192789319999998</v>
+        <v>-0.08648935194259999</v>
       </c>
       <c r="O30" s="0">
         <v>0.076282387300000004</v>
@@ -6490,46 +6537,46 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.074635071260000005</v>
+        <v>0.18929403533399999</v>
       </c>
       <c r="B31" s="0">
-        <v>0.18129715869999999</v>
+        <v>-0.02976755403600001</v>
       </c>
       <c r="C31" s="0">
-        <v>-0.068124624329999994</v>
+        <v>-0.19097107003880001</v>
       </c>
       <c r="D31" s="0">
-        <v>-0.35594292329999999</v>
+        <v>-0.019217983379999998</v>
       </c>
       <c r="E31" s="0">
-        <v>-0.41424499549999999</v>
+        <v>0.24995341966199999</v>
       </c>
       <c r="F31" s="0">
-        <v>0.31539501050000002</v>
+        <v>0.0045223151419999889</v>
       </c>
       <c r="G31" s="0">
-        <v>0.21453353119999999</v>
+        <v>-0.24489715323199998</v>
       </c>
       <c r="H31" s="0">
-        <v>-0.159831271</v>
+        <v>-0.023893723859199988</v>
       </c>
       <c r="I31" s="0">
-        <v>-0.075573040029999997</v>
+        <v>-0.029050380239999986</v>
       </c>
       <c r="J31" s="0">
-        <v>-0.3339285595</v>
+        <v>-0.27623743516999999</v>
       </c>
       <c r="K31" s="0">
-        <v>0.067929079759999997</v>
+        <v>0.091722231073999988</v>
       </c>
       <c r="L31" s="0">
-        <v>-0.65097291930000001</v>
+        <v>-0.43078204609600002</v>
       </c>
       <c r="M31" s="0">
-        <v>0.28302521730000002</v>
+        <v>-0.49073652460000006</v>
       </c>
       <c r="N31" s="0">
-        <v>0.40648804830000002</v>
+        <v>-0.1783430017</v>
       </c>
       <c r="O31" s="0">
         <v>0.14248645030000001</v>
@@ -6702,46 +6749,46 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.56043646680000003</v>
+        <v>0.005728990860000005</v>
       </c>
       <c r="B32" s="0">
-        <v>-0.28328371149999998</v>
+        <v>-0.082030839928000018</v>
       </c>
       <c r="C32" s="0">
-        <v>0.32690989980000001</v>
+        <v>-0.038060549759999993</v>
       </c>
       <c r="D32" s="0">
-        <v>-0.0079426376439999998</v>
+        <v>-0.069806715842000003</v>
       </c>
       <c r="E32" s="0">
-        <v>-0.39337595209999998</v>
+        <v>-0.10970503524000001</v>
       </c>
       <c r="F32" s="0">
-        <v>0.29677808080000001</v>
+        <v>0.11441587527799997</v>
       </c>
       <c r="G32" s="0">
-        <v>0.02504957147</v>
+        <v>0.21854973391999999</v>
       </c>
       <c r="H32" s="0">
-        <v>0.13111757169999999</v>
+        <v>0.08608694057800001</v>
       </c>
       <c r="I32" s="0">
-        <v>-0.31402433769999999</v>
+        <v>-0.092586001283999991</v>
       </c>
       <c r="J32" s="0">
-        <v>-0.84689199820000005</v>
+        <v>0.11103821818000001</v>
       </c>
       <c r="K32" s="0">
-        <v>0.42306953730000002</v>
+        <v>-0.062579285620000022</v>
       </c>
       <c r="L32" s="0">
-        <v>-0.0043088460350000002</v>
+        <v>-0.29370439743799998</v>
       </c>
       <c r="M32" s="0">
-        <v>-0.2846864885</v>
+        <v>-0.36632170084000004</v>
       </c>
       <c r="N32" s="0">
-        <v>-1.217854666</v>
+        <v>0.050292093859999998</v>
       </c>
       <c r="O32" s="0">
         <v>-0.3213862965</v>
@@ -6914,46 +6961,46 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.063242813270000003</v>
+        <v>0.18085321381000002</v>
       </c>
       <c r="B33" s="0">
-        <v>-0.78380432830000002</v>
+        <v>0.065662611326000001</v>
       </c>
       <c r="C33" s="0">
-        <v>-0.41949018529999998</v>
+        <v>0.1136400523</v>
       </c>
       <c r="D33" s="0">
-        <v>0</v>
+        <v>0.16809706485799999</v>
       </c>
       <c r="E33" s="0">
-        <v>-0.27992391519999998</v>
+        <v>-0.063995554553999995</v>
       </c>
       <c r="F33" s="0">
-        <v>-0.1297995871</v>
+        <v>0.31252366030000001</v>
       </c>
       <c r="G33" s="0">
-        <v>-0.65874959509999997</v>
+        <v>0.09058748849999998</v>
       </c>
       <c r="H33" s="0">
-        <v>-0.97750421610000005</v>
+        <v>0.071823532219999972</v>
       </c>
       <c r="I33" s="0">
-        <v>0</v>
+        <v>0.085392520860000015</v>
       </c>
       <c r="J33" s="0">
-        <v>-0.49786993070000002</v>
+        <v>-0.18316417239999999</v>
       </c>
       <c r="K33" s="0">
-        <v>-0.23958965360000001</v>
+        <v>0.082211160399999983</v>
       </c>
       <c r="L33" s="0">
-        <v>-0.28193641250000001</v>
+        <v>-0.036273980720000008</v>
       </c>
       <c r="M33" s="0">
-        <v>-1.642544982</v>
+        <v>-0.12470805567999999</v>
       </c>
       <c r="N33" s="0">
-        <v>0</v>
+        <v>0.16765388352600002</v>
       </c>
       <c r="O33" s="0">
         <v>0.39874933950000002</v>
@@ -7126,46 +7173,46 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.18625208670000001</v>
+        <v>-0.54677096920424995</v>
       </c>
       <c r="B34" s="0">
-        <v>0.54130356170000005</v>
+        <v>-0.5985452294000001</v>
       </c>
       <c r="C34" s="0">
-        <v>0.62794075319999998</v>
+        <v>-0.40782255610000001</v>
       </c>
       <c r="D34" s="0">
-        <v>-0.2353072491</v>
+        <v>-0.50940216969999996</v>
       </c>
       <c r="E34" s="0">
-        <v>-0.46887689729999998</v>
+        <v>-0.43619735461499998</v>
       </c>
       <c r="F34" s="0">
-        <v>0.67908590400000002</v>
+        <v>-0.75164104652999997</v>
       </c>
       <c r="G34" s="0">
-        <v>-0.033653784960000002</v>
+        <v>-0.419181588725</v>
       </c>
       <c r="H34" s="0">
-        <v>0.25939571909999998</v>
+        <v>-0.29570467302500003</v>
       </c>
       <c r="I34" s="0">
-        <v>-0.20999768560000001</v>
+        <v>-0.32780120554999997</v>
       </c>
       <c r="J34" s="0">
-        <v>-0.33705897219999997</v>
+        <v>-0.54224395904999989</v>
       </c>
       <c r="K34" s="0">
-        <v>-0.075875613240000001</v>
+        <v>-0.69523023451499999</v>
       </c>
       <c r="L34" s="0">
-        <v>0.070121311160000005</v>
+        <v>-0.29591579060250001</v>
       </c>
       <c r="M34" s="0">
-        <v>0.29731559359999998</v>
+        <v>-0.024114437024999991</v>
       </c>
       <c r="N34" s="0">
-        <v>-0.19287493310000001</v>
+        <v>-0.0087273348250000056</v>
       </c>
       <c r="O34" s="0">
         <v>0.048692091069999999</v>
@@ -7338,46 +7385,46 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>-0.4023658336</v>
+        <v>0.074979400594000017</v>
       </c>
       <c r="B35" s="0">
-        <v>-0.13795033409999999</v>
+        <v>0.19727106428000002</v>
       </c>
       <c r="C35" s="0">
-        <v>0.54554474990000001</v>
+        <v>-0.125795220102</v>
       </c>
       <c r="D35" s="0">
-        <v>0.83167074699999999</v>
+        <v>-0.25635904096000001</v>
       </c>
       <c r="E35" s="0">
-        <v>0.65521661099999995</v>
+        <v>-0.17787053095200001</v>
       </c>
       <c r="F35" s="0">
-        <v>-0.21402059349999999</v>
+        <v>-0.25095809863599999</v>
       </c>
       <c r="G35" s="0">
-        <v>0.25510148300000002</v>
+        <v>-0.374184857466</v>
       </c>
       <c r="H35" s="0">
-        <v>0.28350043390000002</v>
+        <v>-0.29607404372480001</v>
       </c>
       <c r="I35" s="0">
-        <v>0.93979902260000003</v>
+        <v>-0.27262324618</v>
       </c>
       <c r="J35" s="0">
-        <v>0.68549690640000005</v>
+        <v>-0.31937694002000006</v>
       </c>
       <c r="K35" s="0">
-        <v>-0.38409139320000002</v>
+        <v>0.19747158500599998</v>
       </c>
       <c r="L35" s="0">
-        <v>0.19244599270000001</v>
+        <v>-0.15653823258000002</v>
       </c>
       <c r="M35" s="0">
-        <v>-0.039710037830000003</v>
+        <v>-0.29411398825599999</v>
       </c>
       <c r="N35" s="0">
-        <v>-0.24493661010000001</v>
+        <v>-0.24475923397999999</v>
       </c>
       <c r="O35" s="0">
         <v>0.89730491710000004</v>
@@ -7550,46 +7597,46 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.78949801870000003</v>
+        <v>0.053594512924000005</v>
       </c>
       <c r="B36" s="0">
-        <v>0.076071336559999994</v>
+        <v>-0.051124439947999999</v>
       </c>
       <c r="C36" s="0">
-        <v>-0.43854945550000002</v>
+        <v>-0.10861153241000002</v>
       </c>
       <c r="D36" s="0">
-        <v>0.27983857000000001</v>
+        <v>-0.051590851001999984</v>
       </c>
       <c r="E36" s="0">
-        <v>0.19009589630000001</v>
+        <v>-0.0055875493440000088</v>
       </c>
       <c r="F36" s="0">
-        <v>0.85235150079999999</v>
+        <v>-0.1199719526</v>
       </c>
       <c r="G36" s="0">
-        <v>-0.23082653019999999</v>
+        <v>-0.095385099019999975</v>
       </c>
       <c r="H36" s="0">
-        <v>-1.06890463</v>
+        <v>-0.048468316060000016</v>
       </c>
       <c r="I36" s="0">
-        <v>0.60628836230000005</v>
+        <v>-0.08747142363999999</v>
       </c>
       <c r="J36" s="0">
-        <v>0.7247054973</v>
+        <v>-0.20479173727200001</v>
       </c>
       <c r="K36" s="0">
-        <v>0.65871733619999995</v>
+        <v>-0.177918725394</v>
       </c>
       <c r="L36" s="0">
-        <v>0.14227395370000001</v>
+        <v>-0.081888546125999981</v>
       </c>
       <c r="M36" s="0">
-        <v>-0.68553899340000002</v>
+        <v>-0.1897682389</v>
       </c>
       <c r="N36" s="0">
-        <v>0.7039844649</v>
+        <v>-0.17704627574000004</v>
       </c>
       <c r="O36" s="0">
         <v>1.0403552680000001</v>
@@ -7762,46 +7809,46 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>-0.079088635800000001</v>
+        <v>-0.123288678008</v>
       </c>
       <c r="B37" s="0">
-        <v>-0.47742217310000001</v>
+        <v>-0.13509402279999996</v>
       </c>
       <c r="C37" s="0">
-        <v>-0.67020813189999995</v>
+        <v>-0.0037161644400000248</v>
       </c>
       <c r="D37" s="0">
-        <v>-0.0076945255520000002</v>
+        <v>0.18816483779400001</v>
       </c>
       <c r="E37" s="0">
-        <v>-1.2763579469999999</v>
+        <v>0.57009511828000003</v>
       </c>
       <c r="F37" s="0">
-        <v>-0.3671061088</v>
+        <v>-0.051863792402000009</v>
       </c>
       <c r="G37" s="0">
-        <v>-0.060822541950000003</v>
+        <v>-0.20156523131999998</v>
       </c>
       <c r="H37" s="0">
-        <v>-0.53932239829999995</v>
+        <v>-0.04156272663599999</v>
       </c>
       <c r="I37" s="0">
-        <v>-0.36531482980000002</v>
+        <v>0.101651464796</v>
       </c>
       <c r="J37" s="0">
-        <v>-1.7245826259999999</v>
+        <v>0.019772885900000047</v>
       </c>
       <c r="K37" s="0">
-        <v>-0.88156769199999996</v>
+        <v>-0.20101067134199999</v>
       </c>
       <c r="L37" s="0">
-        <v>-0.098834057719999993</v>
+        <v>-0.10867540471999999</v>
       </c>
       <c r="M37" s="0">
-        <v>-0.63855438050000002</v>
+        <v>-0.097842541519999965</v>
       </c>
       <c r="N37" s="0">
-        <v>-0.9442198919</v>
+        <v>0.052459334680000011</v>
       </c>
       <c r="O37" s="0">
         <v>-1.3300000160000001</v>
@@ -7974,46 +8021,46 @@
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.35299724869999999</v>
+        <v>-0.18490965797999998</v>
       </c>
       <c r="B38" s="0">
-        <v>-1.0335598479999999</v>
+        <v>-0.49720951900600008</v>
       </c>
       <c r="C38" s="0">
-        <v>0.43164379419999999</v>
+        <v>-0.29769711177999997</v>
       </c>
       <c r="D38" s="0">
-        <v>0.037252228739999997</v>
+        <v>-0.14834007681200001</v>
       </c>
       <c r="E38" s="0">
-        <v>-0.26690381229999999</v>
+        <v>0.033126141720000016</v>
       </c>
       <c r="F38" s="0">
-        <v>0.28269765400000002</v>
+        <v>-0.32614679722000001</v>
       </c>
       <c r="G38" s="0">
-        <v>-1.1757186470000001</v>
+        <v>-0.51502502719999999</v>
       </c>
       <c r="H38" s="0">
-        <v>0.5913598229</v>
+        <v>-0.18386410013999999</v>
       </c>
       <c r="I38" s="0">
-        <v>-0.1206642917</v>
+        <v>-0.18432785714000005</v>
       </c>
       <c r="J38" s="0">
-        <v>-0.38655526140000002</v>
+        <v>-0.042545678419999997</v>
       </c>
       <c r="K38" s="0">
-        <v>0.49825924900000002</v>
+        <v>-0.0019222708800000099</v>
       </c>
       <c r="L38" s="0">
-        <v>-1.182780792</v>
+        <v>-0.20804050969999999</v>
       </c>
       <c r="M38" s="0">
-        <v>0.1100671439</v>
+        <v>-0.17834371498000001</v>
       </c>
       <c r="N38" s="0">
-        <v>-0.47883988230000002</v>
+        <v>-0.52360440539499997</v>
       </c>
       <c r="O38" s="0">
         <v>-0.76855981880000002</v>
@@ -8186,46 +8233,46 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.058820912679999997</v>
+        <v>-0.079018746459999983</v>
       </c>
       <c r="B39" s="0">
-        <v>0.31365276889999999</v>
+        <v>-0.022886230190000002</v>
       </c>
       <c r="C39" s="0">
-        <v>0.72399380260000001</v>
+        <v>-0.42896224427999996</v>
       </c>
       <c r="D39" s="0">
-        <v>-0.43021103649999998</v>
+        <v>-0.51894124325999991</v>
       </c>
       <c r="E39" s="0">
-        <v>-0.1454540688</v>
+        <v>-0.32413274662000002</v>
       </c>
       <c r="F39" s="0">
-        <v>0.10801462539999999</v>
+        <v>-0.31939289542000004</v>
       </c>
       <c r="G39" s="0">
-        <v>0.25471883490000002</v>
+        <v>-0.45974004864000007</v>
       </c>
       <c r="H39" s="0">
-        <v>0.4780902736</v>
+        <v>-0.05755932988000001</v>
       </c>
       <c r="I39" s="0">
-        <v>-0.89438626160000001</v>
+        <v>-0.15385719625800001</v>
       </c>
       <c r="J39" s="0">
-        <v>-0.10059546530000001</v>
+        <v>-1.019002661667</v>
       </c>
       <c r="K39" s="0">
-        <v>0.01557353607</v>
+        <v>-0.14911125613999998</v>
       </c>
       <c r="L39" s="0">
-        <v>0.57235860299999997</v>
+        <v>-0.190344388768</v>
       </c>
       <c r="M39" s="0">
-        <v>0.24390418820000001</v>
+        <v>-0.0061762317999999759</v>
       </c>
       <c r="N39" s="0">
-        <v>-1.0663645719999999</v>
+        <v>-0.99760507659200004</v>
       </c>
       <c r="O39" s="0">
         <v>-0.55561698520000002</v>
@@ -8398,46 +8445,46 @@
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.27238300409999999</v>
+        <v>0.044546234977799991</v>
       </c>
       <c r="B40" s="0">
-        <v>-0.21705931349999999</v>
+        <v>-0.29239464002000004</v>
       </c>
       <c r="C40" s="0">
-        <v>-0.68085718890000002</v>
+        <v>-0.13813035779999999</v>
       </c>
       <c r="D40" s="0">
-        <v>0.01153440522</v>
+        <v>-0.20422547971999999</v>
       </c>
       <c r="E40" s="0">
-        <v>-0.37796489760000002</v>
+        <v>-0.090054571946</v>
       </c>
       <c r="F40" s="0">
-        <v>-0.040674477200000003</v>
+        <v>-0.22317560879000001</v>
       </c>
       <c r="G40" s="0">
-        <v>-0.55317555640000005</v>
+        <v>-0.33288367110600003</v>
       </c>
       <c r="H40" s="0">
-        <v>-0.46487829359999999</v>
+        <v>-0.21254725280200004</v>
       </c>
       <c r="I40" s="0">
-        <v>0.72262456500000005</v>
+        <v>0.092162932118000002</v>
       </c>
       <c r="J40" s="0">
-        <v>-0.56674880130000005</v>
+        <v>-0.036085928449999999</v>
       </c>
       <c r="K40" s="0">
-        <v>-0.1848284245</v>
+        <v>-0.17127703424000001</v>
       </c>
       <c r="L40" s="0">
-        <v>-0.92492952070000001</v>
+        <v>-0.21316700250000001</v>
       </c>
       <c r="M40" s="0">
-        <v>-0.1782530739</v>
+        <v>-0.080654440639999964</v>
       </c>
       <c r="N40" s="0">
-        <v>-0.0014187262669999999</v>
+        <v>0.088344273267999957</v>
       </c>
       <c r="O40" s="0">
         <v>-0.63524519300000004</v>
@@ -8610,46 +8657,46 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.21291769460000001</v>
+        <v>-0.014646918958000004</v>
       </c>
       <c r="B41" s="0">
-        <v>0.044684467780000001</v>
+        <v>0.023975867979999999</v>
       </c>
       <c r="C41" s="0">
-        <v>-0.075226481319999997</v>
+        <v>-0.11087946754</v>
       </c>
       <c r="D41" s="0">
-        <v>-0.25433178200000001</v>
+        <v>0.25570558324200005</v>
       </c>
       <c r="E41" s="0">
-        <v>-0.2922323194</v>
+        <v>0.33232963297999996</v>
       </c>
       <c r="F41" s="0">
-        <v>0.40285829750000002</v>
+        <v>-0.22363083304</v>
       </c>
       <c r="G41" s="0">
-        <v>-0.071984355360000002</v>
+        <v>-0.30044315072</v>
       </c>
       <c r="H41" s="0">
-        <v>-0.46437344539999997</v>
+        <v>-0.11066852115799999</v>
       </c>
       <c r="I41" s="0">
-        <v>-0.42988896310000002</v>
+        <v>0.038270254354000006</v>
       </c>
       <c r="J41" s="0">
-        <v>-0.57313719500000004</v>
+        <v>-0.0073841153759999891</v>
       </c>
       <c r="K41" s="0">
-        <v>-0.42229211329999999</v>
+        <v>0.061246014652000004</v>
       </c>
       <c r="L41" s="0">
-        <v>0.2617930839</v>
+        <v>0.25444388062000001</v>
       </c>
       <c r="M41" s="0">
-        <v>-0.191648393</v>
+        <v>0.66085313970000004</v>
       </c>
       <c r="N41" s="0">
-        <v>-0.48689764099999999</v>
+        <v>0.43354971550800003</v>
       </c>
       <c r="O41" s="0">
         <v>-0.67851346629999998</v>
@@ -8822,46 +8869,46 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>-0.69064626920000005</v>
+        <v>0.15737113942999997</v>
       </c>
       <c r="B42" s="0">
-        <v>-0.2052091875</v>
+        <v>-0.22468741876000001</v>
       </c>
       <c r="C42" s="0">
-        <v>-0.34170502609999998</v>
+        <v>-0.245230211354</v>
       </c>
       <c r="D42" s="0">
-        <v>-0.14015750930000001</v>
+        <v>-0.11540902335999999</v>
       </c>
       <c r="E42" s="0">
-        <v>0.25211388870000001</v>
+        <v>-0.014655163539999983</v>
       </c>
       <c r="F42" s="0">
-        <v>-0.63339292390000002</v>
+        <v>-0.28466592010000002</v>
       </c>
       <c r="G42" s="0">
-        <v>-0.31443198220000002</v>
+        <v>-0.48578625629999994</v>
       </c>
       <c r="H42" s="0">
-        <v>-0.32666123749999998</v>
+        <v>-0.38174187932600001</v>
       </c>
       <c r="I42" s="0">
-        <v>-0.79991241420000003</v>
+        <v>-0.14045863832799999</v>
       </c>
       <c r="J42" s="0">
-        <v>0.11862471350000001</v>
+        <v>-0.094802570018000007</v>
       </c>
       <c r="K42" s="0">
-        <v>-0.48950733219999998</v>
+        <v>-0.4014472416</v>
       </c>
       <c r="L42" s="0">
-        <v>0.31099717919999997</v>
+        <v>-0.76899879425999995</v>
       </c>
       <c r="M42" s="0">
-        <v>-0.39657726809999999</v>
+        <v>-0.33994679316600002</v>
       </c>
       <c r="N42" s="0">
-        <v>-0.81481982539999998</v>
+        <v>0.018784179240000042</v>
       </c>
       <c r="O42" s="0">
         <v>0.40902775530000002</v>
@@ -9034,46 +9081,46 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>-0.12529987349999999</v>
+        <v>-0.11767582183400001</v>
       </c>
       <c r="B43" s="0">
-        <v>0.065190056709999999</v>
+        <v>-0.031231405952000003</v>
       </c>
       <c r="C43" s="0">
-        <v>0.16564821800000001</v>
+        <v>0.0089675025400000052</v>
       </c>
       <c r="D43" s="0">
-        <v>0.3474631218</v>
+        <v>-0.36005671962000002</v>
       </c>
       <c r="E43" s="0">
-        <v>-0.24478439269999999</v>
+        <v>-0.42091038926000002</v>
       </c>
       <c r="F43" s="0">
-        <v>0.45654116830000002</v>
+        <v>-0.33935783410000003</v>
       </c>
       <c r="G43" s="0">
-        <v>0.22231943709999999</v>
+        <v>-0.56481906104000001</v>
       </c>
       <c r="H43" s="0">
-        <v>-0.1331431152</v>
+        <v>-0.2834701668704</v>
       </c>
       <c r="I43" s="0">
-        <v>-0.23486403289999999</v>
+        <v>-0.31148566309000003</v>
       </c>
       <c r="J43" s="0">
-        <v>0.1151042464</v>
+        <v>-0.79601889609999998</v>
       </c>
       <c r="K43" s="0">
-        <v>0.87748683490000001</v>
+        <v>0.17617025812000001</v>
       </c>
       <c r="L43" s="0">
-        <v>0.22995536429999999</v>
+        <v>0.19315178982800002</v>
       </c>
       <c r="M43" s="0">
-        <v>0.24387982020000001</v>
+        <v>0.32879459943800005</v>
       </c>
       <c r="N43" s="0">
-        <v>-0.2431576889</v>
+        <v>-0.54788160254000007</v>
       </c>
       <c r="O43" s="0">
         <v>-0.1140072796</v>
@@ -9246,46 +9293,46 @@
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>-0.59487745160000005</v>
+        <v>-0.11181660149999999</v>
       </c>
       <c r="B44" s="0">
-        <v>0.102635083</v>
+        <v>0.050752564259999987</v>
       </c>
       <c r="C44" s="0">
-        <v>0.75182546620000001</v>
+        <v>-0.066731687711999998</v>
       </c>
       <c r="D44" s="0">
-        <v>-0.58419966349999997</v>
+        <v>-0.149339296058</v>
       </c>
       <c r="E44" s="0">
-        <v>-0.47554500119999998</v>
+        <v>-0.038807868016000002</v>
       </c>
       <c r="F44" s="0">
-        <v>-0.82943315419999997</v>
+        <v>-0.28066726425999999</v>
       </c>
       <c r="G44" s="0">
-        <v>-0.028124715429999999</v>
+        <v>-0.34608858147999999</v>
       </c>
       <c r="H44" s="0">
-        <v>0.77503639589999995</v>
+        <v>-0.14239684300399999</v>
       </c>
       <c r="I44" s="0">
-        <v>-0.1645018379</v>
+        <v>0.019098441838000014</v>
       </c>
       <c r="J44" s="0">
-        <v>-0.62407772110000004</v>
+        <v>-0.18115622937999998</v>
       </c>
       <c r="K44" s="0">
-        <v>-0.46684537479999999</v>
+        <v>-0.22152001823799999</v>
       </c>
       <c r="L44" s="0">
-        <v>-0.35911760990000002</v>
+        <v>-0.31678882654039997</v>
       </c>
       <c r="M44" s="0">
-        <v>0.80594074959999995</v>
+        <v>-0.56806312442000007</v>
       </c>
       <c r="N44" s="0">
-        <v>-0.4019674547</v>
+        <v>0.39719347349999995</v>
       </c>
       <c r="O44" s="0">
         <v>-0.56576498959999999</v>
@@ -9458,46 +9505,46 @@
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>-0.015832420520000001</v>
+        <v>0.014861940050000005</v>
       </c>
       <c r="B45" s="0">
-        <v>-0.57728833079999997</v>
+        <v>0.30429007131999997</v>
       </c>
       <c r="C45" s="0">
-        <v>0</v>
+        <v>-0.0822687577</v>
       </c>
       <c r="D45" s="0">
-        <v>-0.31320206649999999</v>
+        <v>-0.35113573510399998</v>
       </c>
       <c r="E45" s="0">
-        <v>-0.27464062140000001</v>
+        <v>-0.26370171232</v>
       </c>
       <c r="F45" s="0">
-        <v>0.50632371399999998</v>
+        <v>-0.34322616180600002</v>
       </c>
       <c r="G45" s="0">
-        <v>-0.74993088510000006</v>
+        <v>0.19752038448000001</v>
       </c>
       <c r="H45" s="0">
-        <v>0</v>
+        <v>0.083051227411999981</v>
       </c>
       <c r="I45" s="0">
-        <v>-0.079594625409999994</v>
+        <v>0.025882105450000005</v>
       </c>
       <c r="J45" s="0">
-        <v>0.2353946831</v>
+        <v>0.23845059935999999</v>
       </c>
       <c r="K45" s="0">
-        <v>0.66919949079999996</v>
+        <v>0.038245261639999986</v>
       </c>
       <c r="L45" s="0">
-        <v>-0.93648640439999997</v>
+        <v>0.020005150229999998</v>
       </c>
       <c r="M45" s="0">
-        <v>0</v>
+        <v>0.089117965899999957</v>
       </c>
       <c r="N45" s="0">
-        <v>-0.40087061619999997</v>
+        <v>-0.055650307500000017</v>
       </c>
       <c r="O45" s="0">
         <v>0.23920347259999999</v>
@@ -9670,46 +9717,46 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>-0.016976506459999999</v>
+        <v>-0.28740094507499997</v>
       </c>
       <c r="B46" s="0">
-        <v>-0.24962140150000001</v>
+        <v>-0.33726335755000003</v>
       </c>
       <c r="C46" s="0">
-        <v>-0.47850041999999998</v>
+        <v>-0.23469229642249997</v>
       </c>
       <c r="D46" s="0">
-        <v>-0.64952191520000002</v>
+        <v>-0.34922469569999998</v>
       </c>
       <c r="E46" s="0">
-        <v>0.039805258060000001</v>
+        <v>-0.20184690566750005</v>
       </c>
       <c r="F46" s="0">
-        <v>-0.064374328460000005</v>
+        <v>-0.36828665354999995</v>
       </c>
       <c r="G46" s="0">
-        <v>0.14877037800000001</v>
+        <v>-0.48221606247500004</v>
       </c>
       <c r="H46" s="0">
-        <v>-0.74069558729999996</v>
+        <v>-0.61026974313500004</v>
       </c>
       <c r="I46" s="0">
-        <v>-0.1531273313</v>
+        <v>-0.2863100515525</v>
       </c>
       <c r="J46" s="0">
-        <v>0.90399015009999995</v>
+        <v>-0.52488054465</v>
       </c>
       <c r="K46" s="0">
-        <v>0.49957220320000001</v>
+        <v>-0.048613286894999996</v>
       </c>
       <c r="L46" s="0">
-        <v>0.1632554896</v>
+        <v>-0.22561817082499996</v>
       </c>
       <c r="M46" s="0">
-        <v>-0.76094635879999994</v>
+        <v>-0.12543797039499999</v>
       </c>
       <c r="N46" s="0">
-        <v>0.22666156509999999</v>
+        <v>-0.37853253183249996</v>
       </c>
       <c r="O46" s="0">
         <v>1.911679589</v>
@@ -9882,46 +9929,46 @@
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.081708992950000003</v>
+        <v>0.15701511676999996</v>
       </c>
       <c r="B47" s="0">
-        <v>0.2219452257</v>
+        <v>0.067622035739999961</v>
       </c>
       <c r="C47" s="0">
-        <v>0</v>
+        <v>0.319473473048</v>
       </c>
       <c r="D47" s="0">
-        <v>0.54012617340000002</v>
+        <v>0.084836738652000004</v>
       </c>
       <c r="E47" s="0">
-        <v>-0.23530649770000001</v>
+        <v>0.17426618428239998</v>
       </c>
       <c r="F47" s="0">
-        <v>0.3395870399</v>
+        <v>0.090303468720000002</v>
       </c>
       <c r="G47" s="0">
-        <v>-0.084602625609999996</v>
+        <v>0.056006818485999997</v>
       </c>
       <c r="H47" s="0">
-        <v>0</v>
+        <v>-0.085058423571999997</v>
       </c>
       <c r="I47" s="0">
-        <v>0.012903597609999999</v>
+        <v>0.010710264979999985</v>
       </c>
       <c r="J47" s="0">
-        <v>-0.39324929870000003</v>
+        <v>0.22257114560399999</v>
       </c>
       <c r="K47" s="0">
-        <v>0.83342734330000001</v>
+        <v>0.54205924492400004</v>
       </c>
       <c r="L47" s="0">
-        <v>0.39337416739999997</v>
+        <v>0.22024200992400003</v>
       </c>
       <c r="M47" s="0">
-        <v>0</v>
+        <v>0.39186679132000002</v>
       </c>
       <c r="N47" s="0">
-        <v>-0.01587095413</v>
+        <v>0.27048909692000001</v>
       </c>
       <c r="O47" s="0">
         <v>0.24858040619999999</v>
@@ -10094,46 +10141,46 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>-0.10434564189999999</v>
+        <v>0.027729544700000011</v>
       </c>
       <c r="B48" s="0">
-        <v>0.56849102569999999</v>
+        <v>0.43302776477499999</v>
       </c>
       <c r="C48" s="0">
-        <v>0</v>
+        <v>0.29206992929999998</v>
       </c>
       <c r="D48" s="0">
-        <v>0.2250711567</v>
+        <v>-0.15221269739000004</v>
       </c>
       <c r="E48" s="0">
-        <v>-0.269089146</v>
+        <v>0.019977268100000001</v>
       </c>
       <c r="F48" s="0">
-        <v>0.86078887410000005</v>
+        <v>-0.18990660947499999</v>
       </c>
       <c r="G48" s="0">
-        <v>0.41461256270000002</v>
+        <v>-0.037314220450000005</v>
       </c>
       <c r="H48" s="0">
-        <v>0</v>
+        <v>-0.15351002766749999</v>
       </c>
       <c r="I48" s="0">
-        <v>0.1944696685</v>
+        <v>-0.065363476562499995</v>
       </c>
       <c r="J48" s="0">
-        <v>-0.074731076610000002</v>
+        <v>0.47497321939999992</v>
       </c>
       <c r="K48" s="0">
-        <v>0.81105249059999995</v>
+        <v>0.56297257725000005</v>
       </c>
       <c r="L48" s="0">
-        <v>0.71560990049999995</v>
+        <v>0.3292233215</v>
       </c>
       <c r="M48" s="0">
-        <v>0</v>
+        <v>0.17086341034750002</v>
       </c>
       <c r="N48" s="0">
-        <v>-0.0092182142809999999</v>
+        <v>-0.073844130872499983</v>
       </c>
       <c r="O48" s="0">
         <v>-0.2301575163</v>
@@ -10306,46 +10353,46 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.2341161471</v>
+        <v>0.33639749337500002</v>
       </c>
       <c r="B49" s="0">
-        <v>0.28113928890000001</v>
+        <v>0.71485658242499994</v>
       </c>
       <c r="C49" s="0">
-        <v>-0.35050148949999999</v>
+        <v>0.68865235725000007</v>
       </c>
       <c r="D49" s="0">
-        <v>-0.4821374699</v>
+        <v>0.043577553472500009</v>
       </c>
       <c r="E49" s="0">
-        <v>0.37597120610000001</v>
+        <v>-0.29535256495000001</v>
       </c>
       <c r="F49" s="0">
-        <v>-0.087528698150000001</v>
+        <v>0.17229771820000001</v>
       </c>
       <c r="G49" s="0">
-        <v>-0.41078686879999998</v>
+        <v>0.16707570667500002</v>
       </c>
       <c r="H49" s="0">
-        <v>-0.13647917239999999</v>
+        <v>0.20399600975500001</v>
       </c>
       <c r="I49" s="0">
-        <v>-0.61846520490000001</v>
+        <v>0.15170704245</v>
       </c>
       <c r="J49" s="0">
-        <v>-0.00325052147</v>
+        <v>-0.12749859107499997</v>
       </c>
       <c r="K49" s="0">
-        <v>0.2294301869</v>
+        <v>0.55131213229999998</v>
       </c>
       <c r="L49" s="0">
-        <v>-0.26031016629999998</v>
+        <v>0.41982698689999998</v>
       </c>
       <c r="M49" s="0">
-        <v>-0.38931280309999999</v>
+        <v>0.43289232827500002</v>
       </c>
       <c r="N49" s="0">
-        <v>-0.49822561999999998</v>
+        <v>0.51729593137499996</v>
       </c>
       <c r="O49" s="0">
         <v>0.53844279559999997</v>
@@ -10518,46 +10565,46 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.069055543959999993</v>
+        <v>0.011674378651999981</v>
       </c>
       <c r="B50" s="0">
-        <v>1.784067265</v>
+        <v>0.13472475465600003</v>
       </c>
       <c r="C50" s="0">
-        <v>0</v>
+        <v>-0.026821156041999999</v>
       </c>
       <c r="D50" s="0">
-        <v>-0.1183358565</v>
+        <v>-0.133557534472</v>
       </c>
       <c r="E50" s="0">
-        <v>-0.29415006510000002</v>
+        <v>0.13531035669159999</v>
       </c>
       <c r="F50" s="0">
-        <v>-0.2672687654</v>
+        <v>0.14565291427200006</v>
       </c>
       <c r="G50" s="0">
-        <v>1.8418207680000001</v>
+        <v>0.083215789200000015</v>
       </c>
       <c r="H50" s="0">
-        <v>0</v>
+        <v>-0.073667310434000016</v>
       </c>
       <c r="I50" s="0">
-        <v>0.52515858630000001</v>
+        <v>-0.26664220623000001</v>
       </c>
       <c r="J50" s="0">
-        <v>-0.1128713111</v>
+        <v>0.059268956219999946</v>
       </c>
       <c r="K50" s="0">
-        <v>0.18017140309999999</v>
+        <v>0.081405785344000017</v>
       </c>
       <c r="L50" s="0">
-        <v>1.0485724489999999</v>
+        <v>0.026916678077999988</v>
       </c>
       <c r="M50" s="0">
-        <v>0</v>
+        <v>0.14716759924</v>
       </c>
       <c r="N50" s="0">
-        <v>0.23258755189999999</v>
+        <v>-0.098824155343</v>
       </c>
       <c r="O50" s="0">
         <v>0.3814151717</v>
@@ -10730,46 +10777,46 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>-0.089017635799999995</v>
+        <v>0.21272562366499997</v>
       </c>
       <c r="B51" s="0">
-        <v>-0.61784582779999997</v>
+        <v>0.42826608150000001</v>
       </c>
       <c r="C51" s="0">
-        <v>0</v>
+        <v>0.090019118049999958</v>
       </c>
       <c r="D51" s="0">
-        <v>-0.51690870339999995</v>
+        <v>-0.13966105214999999</v>
       </c>
       <c r="E51" s="0">
-        <v>-0.66181114730000001</v>
+        <v>-0.3603883536875</v>
       </c>
       <c r="F51" s="0">
-        <v>0.41389955169999998</v>
+        <v>0.12546245485000002</v>
       </c>
       <c r="G51" s="0">
-        <v>-0.32610399979999999</v>
+        <v>0.34769727454999999</v>
       </c>
       <c r="H51" s="0">
-        <v>0</v>
+        <v>0.49760958852499998</v>
       </c>
       <c r="I51" s="0">
-        <v>-0.55579250179999995</v>
+        <v>-0.20305184069999999</v>
       </c>
       <c r="J51" s="0">
-        <v>-0.41361867930000001</v>
+        <v>0.94225027915750004</v>
       </c>
       <c r="K51" s="0">
-        <v>0.27139162760000002</v>
+        <v>0.091124855128750015</v>
       </c>
       <c r="L51" s="0">
-        <v>0.094260979240000001</v>
+        <v>-0.025908035024999998</v>
       </c>
       <c r="M51" s="0">
-        <v>0</v>
+        <v>-0.35865630387499997</v>
       </c>
       <c r="N51" s="0">
-        <v>-0.53155386339999999</v>
+        <v>-0.015729159775000057</v>
       </c>
       <c r="O51" s="0">
         <v>-1.1064945479999999</v>
@@ -10942,46 +10989,46 @@
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>-0.22399058660000001</v>
+        <v>-0.37221578426250002</v>
       </c>
       <c r="B52" s="0">
-        <v>-0.23799334859999999</v>
+        <v>-0.48136101325000002</v>
       </c>
       <c r="C52" s="0">
-        <v>0</v>
+        <v>-0.28055194304999997</v>
       </c>
       <c r="D52" s="0">
-        <v>0.36944743400000002</v>
+        <v>-0.1036324765</v>
       </c>
       <c r="E52" s="0">
-        <v>0</v>
+        <v>-0.58973498704999994</v>
       </c>
       <c r="F52" s="0">
-        <v>-0.049348769629999997</v>
+        <v>-0.34279825207999998</v>
       </c>
       <c r="G52" s="0">
-        <v>0.040255953160000003</v>
+        <v>-0.37953383694999998</v>
       </c>
       <c r="H52" s="0">
-        <v>0</v>
+        <v>-0.25524038388499998</v>
       </c>
       <c r="I52" s="0">
-        <v>0.1609943838</v>
+        <v>-0.27933938784750001</v>
       </c>
       <c r="J52" s="0">
-        <v>0</v>
+        <v>-0.1789779808885</v>
       </c>
       <c r="K52" s="0">
-        <v>0.017415856050000001</v>
+        <v>-0.18660666046250002</v>
       </c>
       <c r="L52" s="0">
-        <v>0.32118366799999998</v>
+        <v>-0.41995574885999998</v>
       </c>
       <c r="M52" s="0">
-        <v>0</v>
+        <v>-0.37914366264749999</v>
       </c>
       <c r="N52" s="0">
-        <v>0.086568230339999996</v>
+        <v>-0.50769239557500001</v>
       </c>
       <c r="O52" s="0">
         <v>0</v>
@@ -11150,6 +11197,50 @@
       </c>
       <c r="BR52" s="0">
         <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>-0.6152199831666666</v>
+      </c>
+      <c r="B53" s="0">
+        <v>-0.48961685188333343</v>
+      </c>
+      <c r="C53" s="0">
+        <v>-0.30313926887000003</v>
+      </c>
+      <c r="D53" s="0">
+        <v>-0.035267152333333336</v>
+      </c>
+      <c r="E53" s="0">
+        <v>-0.60779118873333338</v>
+      </c>
+      <c r="F53" s="0">
+        <v>-0.10968015980000001</v>
+      </c>
+      <c r="G53" s="0">
+        <v>0.11503947892666666</v>
+      </c>
+      <c r="H53" s="0">
+        <v>0.0024838254100000012</v>
+      </c>
+      <c r="I53" s="0">
+        <v>-0.55930822466666663</v>
+      </c>
+      <c r="J53" s="0">
+        <v>-0.27374326789999998</v>
+      </c>
+      <c r="K53" s="0">
+        <v>0.041176115266666681</v>
+      </c>
+      <c r="L53" s="0">
+        <v>-0.75269883013333327</v>
+      </c>
+      <c r="M53" s="0">
+        <v>-0.78019503653333333</v>
+      </c>
+      <c r="N53" s="0">
+        <v>-0.33367815718000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>